<commit_message>
Update Gantt Chart & SOW
</commit_message>
<xml_diff>
--- a/Gantt_project_planner.xlsx
+++ b/Gantt_project_planner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yunyu\Desktop\s\19s1\COMP8715\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yunyu\Desktop\s\19s1\COMP8715\React\Git\energy_storage_rights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454CA75F-4CA1-4738-8587-98F8031B131B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937BBCFD-1695-4209-81DD-333571E28B08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Project Planner</t>
   </si>
@@ -176,10 +176,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Algorithm Brainstroming</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>Setting up platform for Map</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -220,14 +216,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Algorithm deveplment</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete data collection</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Establish basic UI </t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -265,6 +253,14 @@
   </si>
   <si>
     <t xml:space="preserve">Mechine learning </t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Further algorithm deveplment</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Large data collection</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -733,7 +729,7 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -863,15 +859,6 @@
         <bottom style="thin">
           <color theme="7"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
         <vertical/>
         <horizontal/>
       </border>
@@ -1233,10 +1220,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AD33"/>
+  <dimension ref="B1:AD32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1270,7 +1257,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2" s="26"/>
       <c r="J2" s="18" t="s">
@@ -1387,7 +1374,7 @@
     </row>
     <row r="5" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1507,7 +1494,7 @@
     </row>
     <row r="11" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="7">
         <v>3</v>
@@ -1535,8 +1522,12 @@
       <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
       <c r="G12" s="24">
         <v>0</v>
       </c>
@@ -1546,29 +1537,37 @@
         <v>20</v>
       </c>
       <c r="C13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="7">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
       <c r="G13" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8">
         <v>4</v>
       </c>
       <c r="D14" s="7">
-        <v>2</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>5</v>
+      </c>
+      <c r="F14" s="7">
+        <v>3</v>
+      </c>
       <c r="G14" s="24">
         <v>0</v>
       </c>
@@ -1577,21 +1576,25 @@
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>4</v>
       </c>
       <c r="D15" s="7">
         <v>3</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="7">
+        <v>5</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
       <c r="G15" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="2" t="s">
-        <v>24</v>
+      <c r="B16" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="C16" s="7">
         <v>4</v>
@@ -1599,8 +1602,12 @@
       <c r="D16" s="7">
         <v>3</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3</v>
+      </c>
       <c r="G16" s="24">
         <v>0</v>
       </c>
@@ -1615,21 +1622,25 @@
       <c r="D17" s="7">
         <v>3</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7">
+        <v>3</v>
+      </c>
       <c r="G17" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C18" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1653,57 +1664,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="7">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>2</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="24">
+    <row r="20" spans="2:23" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+    </row>
+    <row r="21" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7">
+        <v>6</v>
+      </c>
+      <c r="D21" s="7">
+        <v>3</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:23" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-    </row>
     <row r="22" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1">
         <v>6</v>
       </c>
-      <c r="D22" s="7">
-        <v>3</v>
+      <c r="D22" s="1">
+        <v>6</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1713,13 +1724,13 @@
     </row>
     <row r="23" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1728,14 +1739,14 @@
       </c>
     </row>
     <row r="24" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="1">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
+      <c r="B24" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="7">
+        <v>7</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1751,7 +1762,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1761,7 +1772,7 @@
     </row>
     <row r="26" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C26" s="7">
         <v>7</v>
@@ -1777,10 +1788,10 @@
     </row>
     <row r="27" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
@@ -1793,7 +1804,7 @@
     </row>
     <row r="28" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C28" s="7">
         <v>8</v>
@@ -1809,13 +1820,13 @@
     </row>
     <row r="29" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C29" s="7">
         <v>8</v>
       </c>
       <c r="D29" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1825,13 +1836,13 @@
     </row>
     <row r="30" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="23" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C30" s="7">
         <v>8</v>
       </c>
       <c r="D30" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1839,51 +1850,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="7">
-        <v>8</v>
-      </c>
-      <c r="D31" s="7">
-        <v>4</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-    </row>
-    <row r="33" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="2" t="s">
-        <v>42</v>
+    <row r="31" spans="2:23" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+    </row>
+    <row r="32" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1898,29 +1893,29 @@
     <mergeCell ref="G3:G4"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="H5:W31">
-    <cfRule type="expression" dxfId="17" priority="9">
+  <conditionalFormatting sqref="H5:W30">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="9" priority="20">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1929,7 +1924,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:W32">
+  <conditionalFormatting sqref="H31:W31">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1955,7 +1950,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" xWindow="826" yWindow="371" count="14">
+  <dataValidations xWindow="826" yWindow="371" count="14">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>

</xml_diff>

<commit_message>
add code into master bracnh
</commit_message>
<xml_diff>
--- a/Gantt_project_planner.xlsx
+++ b/Gantt_project_planner.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ChromeDownload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yunyu\Desktop\s\19s1\COMP8715\React\Git\energy_storage_rights-master\energy_storage_rights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525974D4-7678-4248-8364-ED28AEC80787}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78883D94-9503-4242-BB3D-F51D9AA22E11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>Project Planner</t>
   </si>
@@ -304,6 +305,74 @@
   </si>
   <si>
     <t>Third delieverable</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Features</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule Completion Week</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actual Completion Week</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Map base website</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>A map engine is included in a website. Allow user to simply move around the map</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic button include "Home", "News",  "Contact", "About"</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display general information</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allow user to search on the map base on their input</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>A search box on the map allow the user to input the map area they would like to see</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integrate above function on one website</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Side bar available</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Including some dummy button to have a feel of the user interface</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch between differernt base map</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch between solar/wind/water</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch between differernt map data</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Different map layer visualized for differernt energy. Example: wind at 10m, wind at 50m.</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -1378,8 +1447,8 @@
   </sheetPr>
   <dimension ref="B1:AD41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2305,4 +2374,87 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6228FAD-4EEC-42EE-967F-E3561193F516}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implement features on web
</commit_message>
<xml_diff>
--- a/Gantt_project_planner.xlsx
+++ b/Gantt_project_planner.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yunyu\Desktop\s\19s1\COMP8715\React\Git\energy_storage_rights-master\energy_storage_rights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78883D94-9503-4242-BB3D-F51D9AA22E11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BDD95D-81CC-4ABA-9A57-291296FFD88B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Project Planner</t>
   </si>
@@ -305,74 +304,6 @@
   </si>
   <si>
     <t>Third delieverable</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Features</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule Completion Week</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Actual Completion Week</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>A Map base website</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>A map engine is included in a website. Allow user to simply move around the map</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Basic button include "Home", "News",  "Contact", "About"</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Display general information</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Allow user to search on the map base on their input</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>A search box on the map allow the user to input the map area they would like to see</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integrate above function on one website</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Side bar available</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Including some dummy button to have a feel of the user interface</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch between differernt base map</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch between solar/wind/water</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch between differernt map data</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Different map layer visualized for differernt energy. Example: wind at 10m, wind at 50m.</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -1447,8 +1378,8 @@
   </sheetPr>
   <dimension ref="B1:AD41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1953,10 +1884,14 @@
       <c r="D22" s="7">
         <v>1</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="7">
+        <v>7</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
       <c r="G22" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1969,10 +1904,14 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="7">
+        <v>7</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
       <c r="G23" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1985,10 +1924,14 @@
       <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="7">
+        <v>7</v>
+      </c>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
       <c r="G24" s="24">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2001,10 +1944,14 @@
       <c r="D25" s="7">
         <v>2</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7">
+        <v>7</v>
+      </c>
+      <c r="F25" s="7">
+        <v>2</v>
+      </c>
       <c r="G25" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2017,10 +1964,14 @@
       <c r="D26" s="7">
         <v>2</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="7">
+        <v>8</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
       <c r="G26" s="24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2049,10 +2000,14 @@
       <c r="D28" s="7">
         <v>2</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="7">
+        <v>8</v>
+      </c>
+      <c r="F28" s="7">
+        <v>2</v>
+      </c>
       <c r="G28" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2065,10 +2020,14 @@
       <c r="D29" s="7">
         <v>2</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="7">
+        <v>8</v>
+      </c>
+      <c r="F29" s="7">
+        <v>2</v>
+      </c>
       <c r="G29" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2081,10 +2040,14 @@
       <c r="D30" s="7">
         <v>2</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="7">
+        <v>8</v>
+      </c>
+      <c r="F30" s="7">
+        <v>2</v>
+      </c>
       <c r="G30" s="24">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2097,8 +2060,12 @@
       <c r="D31" s="7">
         <v>2</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="7">
+        <v>9</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
       <c r="G31" s="24">
         <v>0</v>
       </c>
@@ -2115,7 +2082,9 @@
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="24"/>
+      <c r="G32" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="23" t="s">
@@ -2129,7 +2098,9 @@
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="24"/>
+      <c r="G33" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="2:23" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="27" t="s">
@@ -2167,6 +2138,9 @@
       <c r="D35" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="G35" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
@@ -2178,6 +2152,9 @@
       <c r="D36" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="G36" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
@@ -2189,6 +2166,9 @@
       <c r="D37" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="G37" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
@@ -2200,6 +2180,9 @@
       <c r="D38" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="G38" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
@@ -2211,6 +2194,9 @@
       <c r="D39" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="G39" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
@@ -2221,6 +2207,9 @@
       </c>
       <c r="D40" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="G40" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:23" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -2374,87 +2363,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6228FAD-4EEC-42EE-967F-E3561193F516}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>